<commit_message>
updated comments, removed dead code, added verbose mode
</commit_message>
<xml_diff>
--- a/evaluations_20211220-164427.xlsx
+++ b/evaluations_20211220-164427.xlsx
@@ -494,10 +494,10 @@
         <v>60</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>48.75</v>
+        <v>46.25</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>1.230769230769231</v>
+        <v>1.297297297297297</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" s="1">
@@ -527,13 +527,13 @@
         </is>
       </c>
       <c r="E3" s="1" t="n">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>48.75</v>
+        <v>46.25</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>1.333333333333333</v>
+        <v>1.621621621621622</v>
       </c>
       <c r="I3" s="1">
         <f>G3*H2</f>
@@ -562,13 +562,13 @@
         </is>
       </c>
       <c r="E4" s="1" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>48.75</v>
+        <v>46.25</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>0.717948717948718</v>
+        <v>0.5405405405405406</v>
       </c>
       <c r="I4" s="1">
         <f>G4*H2</f>
@@ -597,13 +597,13 @@
         </is>
       </c>
       <c r="E5" s="1" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>48.75</v>
+        <v>46.25</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>0.717948717948718</v>
+        <v>0.5405405405405406</v>
       </c>
       <c r="I5" s="1">
         <f>G5*H2</f>
@@ -632,13 +632,13 @@
         </is>
       </c>
       <c r="E6" s="1" t="n">
-        <v>60</v>
+        <v>66.66666666666667</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>50</v>
+        <v>50.00000000000001</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>1.2</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="H6" t="inlineStr"/>
       <c r="I6" s="1">
@@ -668,13 +668,13 @@
         </is>
       </c>
       <c r="E7" s="1" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>50</v>
+        <v>50.00000000000001</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="I7" s="1">
         <f>G7*H6</f>
@@ -703,13 +703,13 @@
         </is>
       </c>
       <c r="E8" s="1" t="n">
-        <v>40</v>
+        <v>33.33333333333334</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>50</v>
+        <v>50.00000000000001</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>0.8</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="I8" s="1">
         <f>G8*H6</f>
@@ -738,13 +738,13 @@
         </is>
       </c>
       <c r="E9" s="1" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>50</v>
+        <v>50.00000000000001</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1">
         <f>G9*H6</f>

</xml_diff>